<commit_message>
Agregué gráfica de libros por año de publicación.
</commit_message>
<xml_diff>
--- a/content/blog/2021-10-28-mi-librero/Librero_Inventario.xlsx
+++ b/content/blog/2021-10-28-mi-librero/Librero_Inventario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanely\Documents\R\Librero_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanely\Documents\R-Sites\personal-site\content\blog\2021-10-28-mi-librero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2B7ACA1-40AF-4171-92DC-8CF37C22C5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF64884-1B0B-4F1F-A010-46B1152597BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21F2696F-EC34-4B1B-8C3F-AC6CB76CA4EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{21F2696F-EC34-4B1B-8C3F-AC6CB76CA4EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Librero" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="345">
   <si>
     <t>ISB</t>
   </si>
@@ -1041,6 +1041,37 @@
   </si>
   <si>
     <t>Fredrick</t>
+  </si>
+  <si>
+    <t>Vladimir Nabokov</t>
+  </si>
+  <si>
+    <t>Cuentos completos</t>
+  </si>
+  <si>
+    <t>Amistad de Juventud</t>
+  </si>
+  <si>
+    <t>Alice Munro</t>
+  </si>
+  <si>
+    <t>Los restos del día</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>El ruiseñor</t>
+  </si>
+  <si>
+    <t>Heartstopper</t>
+  </si>
+  <si>
+    <t>Alice Osimore</t>
+  </si>
+  <si>
+    <t>Yanely Luna 
+Gutiérrez</t>
   </si>
 </sst>
 </file>
@@ -1076,11 +1107,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1100,7 +1134,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1396,15 +1430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468B132F-B023-4A19-854D-A7222F726449}">
-  <dimension ref="A1:O131"/>
+  <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
+      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
@@ -6891,6 +6925,150 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="132" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>336</v>
+      </c>
+      <c r="C132" t="s">
+        <v>335</v>
+      </c>
+      <c r="D132" t="s">
+        <v>130</v>
+      </c>
+      <c r="E132" t="s">
+        <v>255</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132">
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+      <c r="K132" t="s">
+        <v>259</v>
+      </c>
+      <c r="L132">
+        <v>1</v>
+      </c>
+      <c r="N132">
+        <v>4</v>
+      </c>
+      <c r="O132">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="133" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>337</v>
+      </c>
+      <c r="C133" t="s">
+        <v>338</v>
+      </c>
+      <c r="D133" t="s">
+        <v>130</v>
+      </c>
+      <c r="E133" t="s">
+        <v>255</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133" t="s">
+        <v>259</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="O133">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="134" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>339</v>
+      </c>
+      <c r="C134" t="s">
+        <v>252</v>
+      </c>
+      <c r="D134" t="s">
+        <v>340</v>
+      </c>
+      <c r="E134" t="s">
+        <v>255</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134" t="s">
+        <v>259</v>
+      </c>
+      <c r="L134">
+        <v>1</v>
+      </c>
+      <c r="N134">
+        <v>5</v>
+      </c>
+      <c r="O134">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="135" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>341</v>
+      </c>
+      <c r="D135" t="s">
+        <v>130</v>
+      </c>
+      <c r="E135" t="s">
+        <v>214</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+      <c r="K135" t="s">
+        <v>259</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="O135">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="136" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>342</v>
+      </c>
+      <c r="C136" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="137" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B137" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6900,11 +7078,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA648FE7-F17E-42EB-BF3F-C1E8AF65DFDC}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -7041,7 +7219,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7057,12 +7235,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D146D70D91F19B4680F566D740214021" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="35aad5b040085e032151c393fa5e5e4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d30653ad-715d-4403-8e99-b47c2d0d9b53" xmlns:ns4="c1af27c9-bd4c-4c9b-8cc2-0373cc04ffe1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42bfc6b828d730db50487660c0af716f" ns3:_="" ns4:_="">
     <xsd:import namespace="d30653ad-715d-4403-8e99-b47c2d0d9b53"/>
@@ -7233,6 +7405,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B9A6CDD-DE91-4E9F-AB81-E33942B04FB7}">
   <ds:schemaRefs>
@@ -7242,23 +7420,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC4B305-3352-4CE5-8B1D-215C035DCC00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d30653ad-715d-4403-8e99-b47c2d0d9b53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c1af27c9-bd4c-4c9b-8cc2-0373cc04ffe1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD2AB6E1-F057-4A90-8D02-89CAD543589C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7276,4 +7437,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC4B305-3352-4CE5-8B1D-215C035DCC00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d30653ad-715d-4403-8e99-b47c2d0d9b53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c1af27c9-bd4c-4c9b-8cc2-0373cc04ffe1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualización de la sección de proyectos.
</commit_message>
<xml_diff>
--- a/content/blog/2021-10-28-mi-librero/Librero_Inventario.xlsx
+++ b/content/blog/2021-10-28-mi-librero/Librero_Inventario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanely\Documents\R-Sites\personal-site\content\blog\2021-10-28-mi-librero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF64884-1B0B-4F1F-A010-46B1152597BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8CB240-1160-42E7-91A8-3CAF62C02C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{21F2696F-EC34-4B1B-8C3F-AC6CB76CA4EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21F2696F-EC34-4B1B-8C3F-AC6CB76CA4EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Librero" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="375">
   <si>
     <t>ISB</t>
   </si>
@@ -1067,11 +1067,100 @@
     <t>Heartstopper</t>
   </si>
   <si>
-    <t>Alice Osimore</t>
-  </si>
-  <si>
-    <t>Yanely Luna 
-Gutiérrez</t>
+    <t>Kristin Hannah</t>
+  </si>
+  <si>
+    <t>Otra vuelta de tuerca</t>
+  </si>
+  <si>
+    <t>Henry James</t>
+  </si>
+  <si>
+    <t>Penguin Clásicos</t>
+  </si>
+  <si>
+    <t>Juvenil/Romance</t>
+  </si>
+  <si>
+    <t>Las maldiciones</t>
+  </si>
+  <si>
+    <t>Clauidia Piñeiro</t>
+  </si>
+  <si>
+    <t>La lección de August</t>
+  </si>
+  <si>
+    <t>R. J. Palacio</t>
+  </si>
+  <si>
+    <t>V&amp;R</t>
+  </si>
+  <si>
+    <t>Wuthering Heights</t>
+  </si>
+  <si>
+    <t>Penguin Classics</t>
+  </si>
+  <si>
+    <t>Juan Villoro</t>
+  </si>
+  <si>
+    <t>El murmullo de las abejas</t>
+  </si>
+  <si>
+    <t>Sofía Segovia</t>
+  </si>
+  <si>
+    <t>Lumen</t>
+  </si>
+  <si>
+    <t>Dónde estás, mundo bello</t>
+  </si>
+  <si>
+    <t>Miércoles en la noche, en el fin del mundo</t>
+  </si>
+  <si>
+    <t>Hèlén Roux</t>
+  </si>
+  <si>
+    <t>Universidad Nacional Autónoma de México</t>
+  </si>
+  <si>
+    <t>Gatos ilustres</t>
+  </si>
+  <si>
+    <t>Doris Lessing</t>
+  </si>
+  <si>
+    <t>Ficciones</t>
+  </si>
+  <si>
+    <t>Jorge Luis Borges</t>
+  </si>
+  <si>
+    <t>Salvar el fuego</t>
+  </si>
+  <si>
+    <t>Guillermo Arriaga</t>
+  </si>
+  <si>
+    <t>Los siete maridos de Evelyn Hugo</t>
+  </si>
+  <si>
+    <t>Taylor Jenkins Reid</t>
+  </si>
+  <si>
+    <t>Umbriel</t>
+  </si>
+  <si>
+    <t>La bailarina de Auschwitz</t>
+  </si>
+  <si>
+    <t>Edith Eger</t>
+  </si>
+  <si>
+    <t>Alice Oseman</t>
   </si>
 </sst>
 </file>
@@ -1430,12 +1519,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468B132F-B023-4A19-854D-A7222F726449}">
-  <dimension ref="A1:O137"/>
+  <dimension ref="A1:O148"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,10 +2419,13 @@
         <v>259</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
         <v>419</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
       </c>
       <c r="O19">
         <v>2020</v>
@@ -2446,8 +2538,23 @@
       <c r="E22" t="s">
         <v>44</v>
       </c>
+      <c r="F22">
+        <v>2012</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
       <c r="K22" t="s">
         <v>259</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
       </c>
       <c r="M22">
         <v>386</v>
@@ -2628,6 +2735,9 @@
       <c r="L26">
         <v>2</v>
       </c>
+      <c r="M26">
+        <v>539</v>
+      </c>
       <c r="N26">
         <v>5</v>
       </c>
@@ -2663,6 +2773,9 @@
       <c r="K27" t="s">
         <v>259</v>
       </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
       <c r="M27">
         <v>215</v>
       </c>
@@ -2686,6 +2799,9 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
+      <c r="F28">
+        <v>2007</v>
+      </c>
       <c r="G28">
         <v>0</v>
       </c>
@@ -3196,6 +3312,18 @@
       <c r="B40" t="s">
         <v>246</v>
       </c>
+      <c r="C40" t="s">
+        <v>355</v>
+      </c>
+      <c r="D40" t="s">
+        <v>290</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40">
+        <v>2008</v>
+      </c>
       <c r="G40">
         <v>0</v>
       </c>
@@ -3207,6 +3335,12 @@
       </c>
       <c r="K40" t="s">
         <v>259</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>203</v>
       </c>
       <c r="N40">
         <v>3</v>
@@ -3753,6 +3887,9 @@
       <c r="E53" t="s">
         <v>191</v>
       </c>
+      <c r="F53">
+        <v>1815</v>
+      </c>
       <c r="G53">
         <v>0</v>
       </c>
@@ -3767,6 +3904,9 @@
       </c>
       <c r="L53">
         <v>1</v>
+      </c>
+      <c r="M53">
+        <v>498</v>
       </c>
       <c r="N53">
         <v>5</v>
@@ -5136,19 +5276,19 @@
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>159</v>
+        <v>356</v>
       </c>
       <c r="C87" t="s">
-        <v>219</v>
+        <v>357</v>
       </c>
       <c r="D87" t="s">
-        <v>40</v>
+        <v>358</v>
       </c>
       <c r="E87" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F87">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -5163,21 +5303,24 @@
         <v>259</v>
       </c>
       <c r="L87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M87">
-        <v>572</v>
+        <v>481</v>
+      </c>
+      <c r="N87">
+        <v>3</v>
       </c>
       <c r="O87">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
+        <v>219</v>
       </c>
       <c r="D88" t="s">
         <v>40</v>
@@ -5186,7 +5329,7 @@
         <v>211</v>
       </c>
       <c r="F88">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -5201,13 +5344,10 @@
         <v>259</v>
       </c>
       <c r="L88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M88">
-        <v>259</v>
-      </c>
-      <c r="N88">
-        <v>5</v>
+        <v>572</v>
       </c>
       <c r="O88">
         <v>2020</v>
@@ -5215,16 +5355,16 @@
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D89" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E89" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F89">
         <v>2019</v>
@@ -5245,10 +5385,10 @@
         <v>1</v>
       </c>
       <c r="M89">
-        <v>375</v>
+        <v>259</v>
       </c>
       <c r="N89">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O89">
         <v>2020</v>
@@ -5256,19 +5396,19 @@
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C90" t="s">
         <v>156</v>
       </c>
       <c r="D90" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="E90" t="s">
         <v>214</v>
       </c>
       <c r="F90">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -5283,21 +5423,21 @@
         <v>259</v>
       </c>
       <c r="L90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M90">
-        <v>347</v>
+        <v>375</v>
       </c>
       <c r="N90">
         <v>3</v>
       </c>
       <c r="O90">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C91" t="s">
         <v>156</v>
@@ -5306,10 +5446,10 @@
         <v>130</v>
       </c>
       <c r="E91" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F91">
-        <v>2007</v>
+        <v>2015</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5324,33 +5464,33 @@
         <v>259</v>
       </c>
       <c r="L91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M91">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="N91">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O91">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C92" t="s">
-        <v>299</v>
+        <v>156</v>
       </c>
       <c r="D92" t="s">
-        <v>300</v>
+        <v>130</v>
       </c>
       <c r="E92" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F92">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -5368,30 +5508,30 @@
         <v>1</v>
       </c>
       <c r="M92">
-        <v>505</v>
+        <v>364</v>
       </c>
       <c r="N92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O92">
-        <v>2016</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>291</v>
+        <v>160</v>
       </c>
       <c r="C93" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D93" t="s">
         <v>300</v>
       </c>
       <c r="E93" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F93">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -5409,7 +5549,7 @@
         <v>1</v>
       </c>
       <c r="M93">
-        <v>407</v>
+        <v>505</v>
       </c>
       <c r="N93">
         <v>3</v>
@@ -5420,19 +5560,19 @@
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>161</v>
+        <v>291</v>
       </c>
       <c r="C94" t="s">
-        <v>222</v>
+        <v>292</v>
       </c>
       <c r="D94" t="s">
-        <v>241</v>
+        <v>300</v>
       </c>
       <c r="E94" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="F94">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5450,30 +5590,30 @@
         <v>1</v>
       </c>
       <c r="M94">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="N94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O94">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D95" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
       <c r="E95" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F95">
-        <v>1947</v>
+        <v>2008</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -5488,30 +5628,33 @@
         <v>259</v>
       </c>
       <c r="L95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M95">
-        <v>263</v>
+        <v>411</v>
+      </c>
+      <c r="N95">
+        <v>4</v>
       </c>
       <c r="O95">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C96" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="D96" t="s">
-        <v>38</v>
+        <v>286</v>
       </c>
       <c r="E96" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F96">
-        <v>1985</v>
+        <v>1947</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -5526,33 +5669,30 @@
         <v>259</v>
       </c>
       <c r="L96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M96">
-        <v>412</v>
-      </c>
-      <c r="N96">
-        <v>5</v>
+        <v>263</v>
       </c>
       <c r="O96">
-        <v>2021</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>251</v>
+        <v>163</v>
       </c>
       <c r="C97" t="s">
-        <v>252</v>
+        <v>194</v>
       </c>
       <c r="D97" t="s">
-        <v>301</v>
+        <v>38</v>
       </c>
       <c r="E97" t="s">
         <v>224</v>
       </c>
       <c r="F97">
-        <v>2005</v>
+        <v>1985</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -5570,7 +5710,7 @@
         <v>1</v>
       </c>
       <c r="M97">
-        <v>351</v>
+        <v>412</v>
       </c>
       <c r="N97">
         <v>5</v>
@@ -5581,19 +5721,19 @@
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="D98" t="s">
-        <v>127</v>
+        <v>301</v>
       </c>
       <c r="E98" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F98">
-        <v>2017</v>
+        <v>2005</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -5608,13 +5748,13 @@
         <v>259</v>
       </c>
       <c r="L98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M98">
-        <v>290</v>
+        <v>351</v>
       </c>
       <c r="N98">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O98">
         <v>2021</v>
@@ -5622,19 +5762,19 @@
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="C99" t="s">
         <v>195</v>
       </c>
       <c r="D99" t="s">
-        <v>302</v>
+        <v>127</v>
       </c>
       <c r="E99" t="s">
         <v>225</v>
       </c>
       <c r="F99">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5646,16 +5786,16 @@
         <v>0</v>
       </c>
       <c r="K99" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M99">
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="N99">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O99">
         <v>2021</v>
@@ -5663,19 +5803,19 @@
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C100" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D100" t="s">
-        <v>130</v>
+        <v>302</v>
       </c>
       <c r="E100" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F100">
-        <v>1977</v>
+        <v>2014</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -5687,24 +5827,24 @@
         <v>0</v>
       </c>
       <c r="K100" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L100">
         <v>1</v>
       </c>
       <c r="M100">
-        <v>652</v>
+        <v>250</v>
       </c>
       <c r="N100">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O100">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C101" t="s">
         <v>196</v>
@@ -5716,7 +5856,7 @@
         <v>226</v>
       </c>
       <c r="F101">
-        <v>1987</v>
+        <v>1977</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -5734,7 +5874,7 @@
         <v>1</v>
       </c>
       <c r="M101">
-        <v>373</v>
+        <v>652</v>
       </c>
       <c r="N101">
         <v>5</v>
@@ -5745,7 +5885,7 @@
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C102" t="s">
         <v>196</v>
@@ -5757,7 +5897,7 @@
         <v>226</v>
       </c>
       <c r="F102">
-        <v>1981</v>
+        <v>1987</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -5775,18 +5915,18 @@
         <v>1</v>
       </c>
       <c r="M102">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="N102">
         <v>5</v>
       </c>
       <c r="O102">
-        <v>2018</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C103" t="s">
         <v>196</v>
@@ -5795,10 +5935,10 @@
         <v>130</v>
       </c>
       <c r="E103" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="F103">
-        <v>2014</v>
+        <v>1981</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -5816,30 +5956,30 @@
         <v>1</v>
       </c>
       <c r="M103">
-        <v>492</v>
+        <v>393</v>
       </c>
       <c r="N103">
         <v>5</v>
       </c>
       <c r="O103">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C104" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="D104" t="s">
         <v>130</v>
       </c>
       <c r="E104" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="F104">
-        <v>1979</v>
+        <v>2014</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5854,13 +5994,13 @@
         <v>259</v>
       </c>
       <c r="L104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M104">
-        <v>469</v>
+        <v>492</v>
       </c>
       <c r="N104">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O104">
         <v>2020</v>
@@ -5868,19 +6008,19 @@
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C105" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D105" t="s">
-        <v>287</v>
+        <v>130</v>
       </c>
       <c r="E105" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F105">
-        <v>2007</v>
+        <v>1979</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -5895,33 +6035,33 @@
         <v>259</v>
       </c>
       <c r="L105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M105">
-        <v>279</v>
+        <v>469</v>
       </c>
       <c r="N105">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O105">
-        <v>2018</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C106" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="D106" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="E106" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="F106">
-        <v>1984</v>
+        <v>2007</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5939,18 +6079,18 @@
         <v>1</v>
       </c>
       <c r="M106">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="N106">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O106">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C107" t="s">
         <v>197</v>
@@ -5959,10 +6099,10 @@
         <v>303</v>
       </c>
       <c r="E107" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F107">
-        <v>1998</v>
+        <v>1984</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5980,10 +6120,10 @@
         <v>1</v>
       </c>
       <c r="M107">
-        <v>178</v>
+        <v>327</v>
       </c>
       <c r="N107">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O107">
         <v>2020</v>
@@ -5991,10 +6131,10 @@
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C108" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
       <c r="D108" t="s">
         <v>303</v>
@@ -6003,7 +6143,7 @@
         <v>211</v>
       </c>
       <c r="F108">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -6018,30 +6158,33 @@
         <v>259</v>
       </c>
       <c r="L108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M108">
-        <v>248</v>
+        <v>178</v>
+      </c>
+      <c r="N108">
+        <v>3</v>
       </c>
       <c r="O108">
-        <v>2016</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C109" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D109" t="s">
-        <v>130</v>
+        <v>303</v>
       </c>
       <c r="E109" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F109">
-        <v>2006</v>
+        <v>2001</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -6059,30 +6202,27 @@
         <v>0</v>
       </c>
       <c r="M109">
-        <v>491</v>
-      </c>
-      <c r="N109">
-        <v>3</v>
+        <v>248</v>
       </c>
       <c r="O109">
-        <v>2020</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>253</v>
+        <v>174</v>
       </c>
       <c r="C110" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="D110" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E110" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="F110">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -6097,36 +6237,36 @@
         <v>259</v>
       </c>
       <c r="L110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M110">
-        <v>253</v>
+        <v>491</v>
       </c>
       <c r="N110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O110">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>175</v>
+        <v>253</v>
       </c>
       <c r="C111" t="s">
-        <v>198</v>
+        <v>254</v>
       </c>
       <c r="D111" t="s">
-        <v>304</v>
+        <v>53</v>
       </c>
       <c r="E111" t="s">
         <v>255</v>
       </c>
       <c r="F111">
-        <v>2019</v>
+        <v>2001</v>
       </c>
       <c r="G111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -6135,16 +6275,16 @@
         <v>0</v>
       </c>
       <c r="K111" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L111">
         <v>1</v>
       </c>
       <c r="M111">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="N111">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O111">
         <v>2021</v>
@@ -6152,10 +6292,10 @@
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>256</v>
+        <v>359</v>
       </c>
       <c r="C112" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D112" t="s">
         <v>53</v>
@@ -6164,10 +6304,10 @@
         <v>255</v>
       </c>
       <c r="F112">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -6176,16 +6316,16 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L112">
         <v>1</v>
       </c>
       <c r="M112">
-        <v>242</v>
+        <v>326</v>
       </c>
       <c r="N112">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O112">
         <v>2021</v>
@@ -6193,22 +6333,22 @@
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D113" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E113" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="F113">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -6217,39 +6357,39 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L113">
         <v>1</v>
       </c>
       <c r="M113">
-        <v>253</v>
+        <v>310</v>
       </c>
       <c r="N113">
         <v>4</v>
       </c>
       <c r="O113">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>177</v>
+        <v>256</v>
       </c>
       <c r="C114" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="D114" t="s">
-        <v>267</v>
+        <v>53</v>
       </c>
       <c r="E114" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="F114">
-        <v>1924</v>
+        <v>2019</v>
       </c>
       <c r="G114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -6258,33 +6398,36 @@
         <v>0</v>
       </c>
       <c r="K114" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M114">
-        <v>93</v>
+        <v>242</v>
+      </c>
+      <c r="N114">
+        <v>4</v>
       </c>
       <c r="O114">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="115" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="C115" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D115" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E115" t="s">
         <v>232</v>
       </c>
       <c r="F115">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -6293,16 +6436,19 @@
         <v>1</v>
       </c>
       <c r="J115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K115" t="s">
         <v>259</v>
       </c>
       <c r="L115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M115">
-        <v>127</v>
+        <v>253</v>
+      </c>
+      <c r="N115">
+        <v>4</v>
       </c>
       <c r="O115">
         <v>2020</v>
@@ -6310,19 +6456,19 @@
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="C116" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="D116" t="s">
-        <v>59</v>
+        <v>267</v>
       </c>
       <c r="E116" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F116">
-        <v>2019</v>
+        <v>1924</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -6340,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="M116">
-        <v>319</v>
+        <v>93</v>
       </c>
       <c r="O116">
         <v>2020</v>
@@ -6348,19 +6494,19 @@
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="C117" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="D117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E117" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F117">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -6369,7 +6515,7 @@
         <v>1</v>
       </c>
       <c r="J117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K117" t="s">
         <v>259</v>
@@ -6378,7 +6524,7 @@
         <v>0</v>
       </c>
       <c r="M117">
-        <v>349</v>
+        <v>127</v>
       </c>
       <c r="O117">
         <v>2020</v>
@@ -6386,16 +6532,16 @@
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C118" t="s">
-        <v>308</v>
+        <v>234</v>
       </c>
       <c r="D118" t="s">
-        <v>309</v>
+        <v>59</v>
       </c>
       <c r="E118" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F118">
         <v>2019</v>
@@ -6416,7 +6562,7 @@
         <v>0</v>
       </c>
       <c r="M118">
-        <v>236</v>
+        <v>319</v>
       </c>
       <c r="O118">
         <v>2020</v>
@@ -6424,19 +6570,19 @@
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C119" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D119" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E119" t="s">
         <v>235</v>
       </c>
       <c r="F119">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -6454,7 +6600,7 @@
         <v>0</v>
       </c>
       <c r="M119">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="O119">
         <v>2020</v>
@@ -6462,25 +6608,25 @@
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>284</v>
+        <v>204</v>
       </c>
       <c r="C120" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="D120" t="s">
-        <v>40</v>
+        <v>309</v>
       </c>
       <c r="E120" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="F120">
-        <v>1980</v>
+        <v>2019</v>
       </c>
       <c r="G120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J120">
         <v>0</v>
@@ -6492,27 +6638,27 @@
         <v>0</v>
       </c>
       <c r="M120">
-        <v>513</v>
+        <v>236</v>
       </c>
       <c r="O120">
-        <v>2010</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>310</v>
+        <v>205</v>
       </c>
       <c r="C121" t="s">
-        <v>311</v>
+        <v>238</v>
       </c>
       <c r="D121" t="s">
-        <v>286</v>
+        <v>314</v>
       </c>
       <c r="E121" t="s">
         <v>235</v>
       </c>
       <c r="F121">
-        <v>1991</v>
+        <v>2015</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -6530,7 +6676,7 @@
         <v>0</v>
       </c>
       <c r="M121">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="O121">
         <v>2020</v>
@@ -6538,25 +6684,25 @@
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C122" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
       <c r="D122" t="s">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="E122" t="s">
-        <v>235</v>
+        <v>10</v>
       </c>
       <c r="F122">
-        <v>2017</v>
+        <v>1980</v>
       </c>
       <c r="G122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J122">
         <v>0</v>
@@ -6565,33 +6711,30 @@
         <v>259</v>
       </c>
       <c r="L122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M122">
-        <v>249</v>
-      </c>
-      <c r="N122">
-        <v>4</v>
+        <v>513</v>
       </c>
       <c r="O122">
-        <v>2020</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C123" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D123" t="s">
-        <v>50</v>
+        <v>286</v>
       </c>
       <c r="E123" t="s">
         <v>235</v>
       </c>
       <c r="F123">
-        <v>1997</v>
+        <v>1991</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -6606,33 +6749,30 @@
         <v>259</v>
       </c>
       <c r="L123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M123">
-        <v>153</v>
-      </c>
-      <c r="N123">
-        <v>3</v>
+        <v>243</v>
       </c>
       <c r="O123">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C124" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D124" t="s">
-        <v>50</v>
+        <v>286</v>
       </c>
       <c r="E124" t="s">
         <v>235</v>
       </c>
       <c r="F124">
-        <v>1999</v>
+        <v>2017</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -6647,10 +6787,13 @@
         <v>259</v>
       </c>
       <c r="L124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M124">
-        <v>222</v>
+        <v>249</v>
+      </c>
+      <c r="N124">
+        <v>4</v>
       </c>
       <c r="O124">
         <v>2020</v>
@@ -6658,19 +6801,19 @@
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C125" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D125" t="s">
-        <v>320</v>
+        <v>50</v>
       </c>
       <c r="E125" t="s">
         <v>235</v>
       </c>
       <c r="F125">
-        <v>2007</v>
+        <v>1997</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -6685,36 +6828,39 @@
         <v>259</v>
       </c>
       <c r="L125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M125">
-        <v>247</v>
+        <v>153</v>
+      </c>
+      <c r="N125">
+        <v>3</v>
       </c>
       <c r="O125">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C126" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D126" t="s">
-        <v>323</v>
+        <v>50</v>
       </c>
       <c r="E126" t="s">
         <v>235</v>
       </c>
       <c r="F126">
-        <v>2011</v>
+        <v>1999</v>
       </c>
       <c r="G126">
         <v>0</v>
       </c>
       <c r="H126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J126">
         <v>0</v>
@@ -6723,30 +6869,33 @@
         <v>259</v>
       </c>
       <c r="L126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M126">
-        <v>206</v>
+        <v>222</v>
+      </c>
+      <c r="N126">
+        <v>3</v>
       </c>
       <c r="O126">
-        <v>2018</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C127" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D127" t="s">
-        <v>130</v>
+        <v>320</v>
       </c>
       <c r="E127" t="s">
         <v>235</v>
       </c>
       <c r="F127">
-        <v>1981</v>
+        <v>2007</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -6761,39 +6910,36 @@
         <v>259</v>
       </c>
       <c r="L127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M127">
-        <v>292</v>
-      </c>
-      <c r="N127">
-        <v>4</v>
+        <v>247</v>
       </c>
       <c r="O127">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C128" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D128" t="s">
-        <v>130</v>
+        <v>323</v>
       </c>
       <c r="E128" t="s">
         <v>235</v>
       </c>
       <c r="F128">
-        <v>218</v>
+        <v>2011</v>
       </c>
       <c r="G128">
         <v>0</v>
       </c>
       <c r="H128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J128">
         <v>0</v>
@@ -6805,24 +6951,27 @@
         <v>0</v>
       </c>
       <c r="M128">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="O128">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="129" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C129" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D129" t="s">
-        <v>330</v>
+        <v>130</v>
       </c>
       <c r="E129" t="s">
-        <v>255</v>
+        <v>235</v>
+      </c>
+      <c r="F129">
+        <v>1981</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -6837,27 +6986,33 @@
         <v>259</v>
       </c>
       <c r="L129">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="M129">
+        <v>292</v>
+      </c>
+      <c r="N129">
+        <v>4</v>
       </c>
       <c r="O129">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="130" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>295</v>
+        <v>326</v>
       </c>
       <c r="C130" t="s">
-        <v>254</v>
+        <v>327</v>
       </c>
       <c r="D130" t="s">
-        <v>331</v>
+        <v>130</v>
       </c>
       <c r="E130" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="F130">
-        <v>2017</v>
+        <v>218</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -6869,36 +7024,33 @@
         <v>0</v>
       </c>
       <c r="K130" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M130">
-        <v>321</v>
-      </c>
-      <c r="N130">
-        <v>5</v>
+        <v>218</v>
       </c>
       <c r="O130">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="131" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C131" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D131" t="s">
-        <v>287</v>
+        <v>330</v>
       </c>
       <c r="E131" t="s">
         <v>255</v>
       </c>
       <c r="F131">
-        <v>2006</v>
+        <v>2017</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -6913,10 +7065,10 @@
         <v>259</v>
       </c>
       <c r="L131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M131">
-        <v>364</v>
+        <v>283</v>
       </c>
       <c r="N131">
         <v>4</v>
@@ -6927,17 +7079,20 @@
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>336</v>
+        <v>295</v>
       </c>
       <c r="C132" t="s">
-        <v>335</v>
+        <v>254</v>
       </c>
       <c r="D132" t="s">
-        <v>130</v>
+        <v>331</v>
       </c>
       <c r="E132" t="s">
         <v>255</v>
       </c>
+      <c r="F132">
+        <v>2017</v>
+      </c>
       <c r="G132">
         <v>0</v>
       </c>
@@ -6948,13 +7103,16 @@
         <v>0</v>
       </c>
       <c r="K132" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L132">
         <v>1</v>
       </c>
+      <c r="M132">
+        <v>321</v>
+      </c>
       <c r="N132">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O132">
         <v>2021</v>
@@ -6962,17 +7120,20 @@
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C133" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D133" t="s">
-        <v>130</v>
+        <v>287</v>
       </c>
       <c r="E133" t="s">
         <v>255</v>
       </c>
+      <c r="F133">
+        <v>2006</v>
+      </c>
       <c r="G133">
         <v>0</v>
       </c>
@@ -6986,7 +7147,13 @@
         <v>259</v>
       </c>
       <c r="L133">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="M133">
+        <v>364</v>
+      </c>
+      <c r="N133">
+        <v>4</v>
       </c>
       <c r="O133">
         <v>2021</v>
@@ -6994,22 +7161,25 @@
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C134" t="s">
-        <v>252</v>
+        <v>335</v>
       </c>
       <c r="D134" t="s">
-        <v>340</v>
+        <v>130</v>
       </c>
       <c r="E134" t="s">
         <v>255</v>
       </c>
+      <c r="F134">
+        <v>2017</v>
+      </c>
       <c r="G134">
         <v>0</v>
       </c>
       <c r="H134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J134">
         <v>0</v>
@@ -7020,8 +7190,11 @@
       <c r="L134">
         <v>1</v>
       </c>
+      <c r="M134">
+        <v>792</v>
+      </c>
       <c r="N134">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O134">
         <v>2021</v>
@@ -7029,19 +7202,25 @@
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>341</v>
+        <v>337</v>
+      </c>
+      <c r="C135" t="s">
+        <v>338</v>
       </c>
       <c r="D135" t="s">
         <v>130</v>
       </c>
       <c r="E135" t="s">
-        <v>214</v>
+        <v>255</v>
+      </c>
+      <c r="F135">
+        <v>1990</v>
       </c>
       <c r="G135">
         <v>0</v>
       </c>
       <c r="H135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J135">
         <v>0</v>
@@ -7051,6 +7230,12 @@
       </c>
       <c r="L135">
         <v>0</v>
+      </c>
+      <c r="M135">
+        <v>319</v>
+      </c>
+      <c r="N135">
+        <v>5</v>
       </c>
       <c r="O135">
         <v>2021</v>
@@ -7058,15 +7243,520 @@
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
+        <v>339</v>
+      </c>
+      <c r="C136" t="s">
+        <v>252</v>
+      </c>
+      <c r="D136" t="s">
+        <v>340</v>
+      </c>
+      <c r="E136" t="s">
+        <v>255</v>
+      </c>
+      <c r="F136">
+        <v>1989</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+      <c r="K136" t="s">
+        <v>259</v>
+      </c>
+      <c r="L136">
+        <v>1</v>
+      </c>
+      <c r="M136">
+        <v>253</v>
+      </c>
+      <c r="N136">
+        <v>5</v>
+      </c>
+      <c r="O136">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="137" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>341</v>
+      </c>
+      <c r="C137" t="s">
+        <v>343</v>
+      </c>
+      <c r="D137" t="s">
+        <v>130</v>
+      </c>
+      <c r="E137" t="s">
+        <v>214</v>
+      </c>
+      <c r="F137">
+        <v>2015</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137" t="s">
+        <v>259</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137">
+        <v>607</v>
+      </c>
+      <c r="O137">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="138" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
         <v>342</v>
       </c>
-      <c r="C136" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="137" spans="2:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="B137" s="3" t="s">
+      <c r="C138" t="s">
+        <v>374</v>
+      </c>
+      <c r="D138" t="s">
+        <v>352</v>
+      </c>
+      <c r="E138" t="s">
+        <v>347</v>
+      </c>
+      <c r="F138">
+        <v>2020</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+      <c r="K138" t="s">
+        <v>259</v>
+      </c>
+      <c r="L138">
+        <v>1</v>
+      </c>
+      <c r="M138">
+        <v>263</v>
+      </c>
+      <c r="N138">
+        <v>5</v>
+      </c>
+      <c r="O138">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="139" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B139" s="3" t="s">
         <v>344</v>
+      </c>
+      <c r="C139" t="s">
+        <v>345</v>
+      </c>
+      <c r="D139" t="s">
+        <v>346</v>
+      </c>
+      <c r="E139" t="s">
+        <v>102</v>
+      </c>
+      <c r="F139">
+        <v>2019</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139" t="s">
+        <v>259</v>
+      </c>
+      <c r="L139">
+        <v>1</v>
+      </c>
+      <c r="M139">
+        <v>255</v>
+      </c>
+      <c r="N139">
+        <v>4</v>
+      </c>
+      <c r="O139">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="140" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>348</v>
+      </c>
+      <c r="C140" t="s">
+        <v>349</v>
+      </c>
+      <c r="D140" t="s">
+        <v>127</v>
+      </c>
+      <c r="E140" t="s">
+        <v>209</v>
+      </c>
+      <c r="F140">
+        <v>2017</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140" t="s">
+        <v>259</v>
+      </c>
+      <c r="L140">
+        <v>0</v>
+      </c>
+      <c r="M140">
+        <v>316</v>
+      </c>
+      <c r="O140">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="141" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>350</v>
+      </c>
+      <c r="C141" t="s">
+        <v>351</v>
+      </c>
+      <c r="D141" t="s">
+        <v>82</v>
+      </c>
+      <c r="E141" t="s">
+        <v>80</v>
+      </c>
+      <c r="F141">
+        <v>2013</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141" t="s">
+        <v>259</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+      <c r="M141">
+        <v>416</v>
+      </c>
+      <c r="O141">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="142" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>353</v>
+      </c>
+      <c r="C142" t="s">
+        <v>135</v>
+      </c>
+      <c r="D142" t="s">
+        <v>354</v>
+      </c>
+      <c r="E142" t="s">
+        <v>191</v>
+      </c>
+      <c r="F142">
+        <v>1847</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142" t="s">
+        <v>260</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+      <c r="M142">
+        <v>359</v>
+      </c>
+      <c r="O142">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="143" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>360</v>
+      </c>
+      <c r="C143" t="s">
+        <v>361</v>
+      </c>
+      <c r="D143" t="s">
+        <v>362</v>
+      </c>
+      <c r="E143" t="s">
+        <v>255</v>
+      </c>
+      <c r="F143">
+        <v>2007</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143" t="s">
+        <v>259</v>
+      </c>
+      <c r="L143">
+        <v>1</v>
+      </c>
+      <c r="M143">
+        <v>216</v>
+      </c>
+      <c r="N143">
+        <v>4</v>
+      </c>
+      <c r="O143">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="144" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>363</v>
+      </c>
+      <c r="C144" t="s">
+        <v>364</v>
+      </c>
+      <c r="D144" t="s">
+        <v>53</v>
+      </c>
+      <c r="E144" t="s">
+        <v>255</v>
+      </c>
+      <c r="F144">
+        <v>2019</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+      <c r="K144" t="s">
+        <v>259</v>
+      </c>
+      <c r="L144">
+        <v>1</v>
+      </c>
+      <c r="M144">
+        <v>160</v>
+      </c>
+      <c r="N144">
+        <v>4</v>
+      </c>
+      <c r="O144">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="145" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>365</v>
+      </c>
+      <c r="C145" t="s">
+        <v>366</v>
+      </c>
+      <c r="D145" t="s">
+        <v>130</v>
+      </c>
+      <c r="E145" t="s">
+        <v>211</v>
+      </c>
+      <c r="F145">
+        <v>2011</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145" t="s">
+        <v>259</v>
+      </c>
+      <c r="L145">
+        <v>1</v>
+      </c>
+      <c r="M145">
+        <v>221</v>
+      </c>
+      <c r="N145">
+        <v>5</v>
+      </c>
+      <c r="O145">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="146" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>367</v>
+      </c>
+      <c r="C146" t="s">
+        <v>368</v>
+      </c>
+      <c r="D146" t="s">
+        <v>127</v>
+      </c>
+      <c r="E146" t="s">
+        <v>211</v>
+      </c>
+      <c r="F146">
+        <v>2020</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146" t="s">
+        <v>259</v>
+      </c>
+      <c r="L146">
+        <v>1</v>
+      </c>
+      <c r="M146">
+        <v>659</v>
+      </c>
+      <c r="N146">
+        <v>4</v>
+      </c>
+      <c r="O146">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="147" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>369</v>
+      </c>
+      <c r="C147" t="s">
+        <v>370</v>
+      </c>
+      <c r="D147" t="s">
+        <v>371</v>
+      </c>
+      <c r="E147" t="s">
+        <v>255</v>
+      </c>
+      <c r="F147">
+        <v>2017</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147" t="s">
+        <v>259</v>
+      </c>
+      <c r="L147">
+        <v>1</v>
+      </c>
+      <c r="M147">
+        <v>380</v>
+      </c>
+      <c r="N147">
+        <v>4</v>
+      </c>
+      <c r="O147">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="148" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>372</v>
+      </c>
+      <c r="C148" t="s">
+        <v>373</v>
+      </c>
+      <c r="D148" t="s">
+        <v>40</v>
+      </c>
+      <c r="E148" t="s">
+        <v>220</v>
+      </c>
+      <c r="F148">
+        <v>2017</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="K148" t="s">
+        <v>259</v>
+      </c>
+      <c r="L148">
+        <v>0</v>
+      </c>
+      <c r="M148">
+        <v>412</v>
+      </c>
+      <c r="O148">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -7078,7 +7768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA648FE7-F17E-42EB-BF3F-C1E8AF65DFDC}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -7235,6 +7925,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D146D70D91F19B4680F566D740214021" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="35aad5b040085e032151c393fa5e5e4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d30653ad-715d-4403-8e99-b47c2d0d9b53" xmlns:ns4="c1af27c9-bd4c-4c9b-8cc2-0373cc04ffe1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42bfc6b828d730db50487660c0af716f" ns3:_="" ns4:_="">
     <xsd:import namespace="d30653ad-715d-4403-8e99-b47c2d0d9b53"/>
@@ -7405,12 +8101,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B9A6CDD-DE91-4E9F-AB81-E33942B04FB7}">
   <ds:schemaRefs>
@@ -7420,6 +8110,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC4B305-3352-4CE5-8B1D-215C035DCC00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d30653ad-715d-4403-8e99-b47c2d0d9b53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c1af27c9-bd4c-4c9b-8cc2-0373cc04ffe1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD2AB6E1-F057-4A90-8D02-89CAD543589C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7437,21 +8144,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC4B305-3352-4CE5-8B1D-215C035DCC00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d30653ad-715d-4403-8e99-b47c2d0d9b53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c1af27c9-bd4c-4c9b-8cc2-0373cc04ffe1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>